<commit_message>
Added the column sNo in all the datasheets so as to fetch the current dataset number at runtime
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/oneWayFlightSearch.xlsx
+++ b/src/test/resources/datasheets/oneWayFlightSearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\MultiAppPOM\multiApp\src\test\resources\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6446F619-CD93-4407-AD9C-1AF4866D1D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1E3D33-322D-48A5-B583-DA7543F0B8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>sourceCity</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>sNo</t>
   </si>
 </sst>
 </file>
@@ -392,66 +395,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>